<commit_message>
CRUD working for library on frontend
</commit_message>
<xml_diff>
--- a/ScopeofWork/Project1FrontEndLayout.xlsx
+++ b/ScopeofWork/Project1FrontEndLayout.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rishi\cs\Skillstorm\Project1InventoryManagementSystem\ScopeofWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AFCEF8-F1AD-4BCC-99A8-0CE0E8066DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C924F2-9834-41FB-BCF8-8D3EAFCD2E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{376300D7-22C6-47C5-BA03-D84FFFF74DCF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{376300D7-22C6-47C5-BA03-D84FFFF74DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Header</t>
   </si>
@@ -51,12 +52,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Titles</t>
-  </si>
-  <si>
-    <t>asdf,asdf,asdf…</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
@@ -127,6 +122,21 @@
   </si>
   <si>
     <t>[transfer to another library]</t>
+  </si>
+  <si>
+    <t>Remove commented out code from model classes</t>
+  </si>
+  <si>
+    <t>Remove commented out style.css</t>
+  </si>
+  <si>
+    <t>Add neat quality frequent comments THROUGHOUT</t>
+  </si>
+  <si>
+    <t>Add modals for deletes</t>
+  </si>
+  <si>
+    <t>Add form validation to disallow empty library entries</t>
   </si>
 </sst>
 </file>
@@ -162,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +197,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -278,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -324,6 +340,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911E330A-F050-4A9A-BA29-DE4B56D4F7D4}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:K7"/>
+    <sheetView topLeftCell="B1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +743,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -753,7 +770,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E7" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -774,67 +791,56 @@
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="J8" s="13"/>
       <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E12" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -845,7 +851,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E13" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -856,7 +862,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D16" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
@@ -866,12 +872,12 @@
       <c r="J16" s="14"/>
       <c r="K16" s="15"/>
       <c r="L16" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D17" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -884,39 +890,39 @@
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D18" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I18" s="16"/>
       <c r="J18" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J19" s="1">
         <v>2007</v>
@@ -928,21 +934,21 @@
         <v>2</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J20" s="1">
         <v>2007</v>
@@ -954,21 +960,21 @@
         <v>5</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J21" s="1">
         <v>2007</v>
@@ -980,12 +986,12 @@
         <v>6</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -998,7 +1004,7 @@
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D23" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1009,7 +1015,7 @@
       <c r="K23" s="10"/>
       <c r="L23" s="11"/>
       <c r="M23" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1033,4 +1039,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF17B7BE-CB9B-4A4D-8A8F-B518B26CE959}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>